<commit_message>
Test Suite xlsx sheet
</commit_message>
<xml_diff>
--- a/resources/testdata/TestSuite.xlsx
+++ b/resources/testdata/TestSuite.xlsx
@@ -34,13 +34,13 @@
     <t>Y</t>
   </si>
   <si>
+    <t>LoginTestCases</t>
+  </si>
+  <si>
+    <t>LoginTestCases1</t>
+  </si>
+  <si>
     <t>N</t>
-  </si>
-  <si>
-    <t>LoginTestCases</t>
-  </si>
-  <si>
-    <t>LoginTestCases1</t>
   </si>
 </sst>
 </file>
@@ -392,12 +392,12 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" customWidth="1"/>
     <col min="2" max="2" width="24.42578125" customWidth="1"/>
     <col min="3" max="3" width="29.28515625" customWidth="1"/>
   </cols>
@@ -415,24 +415,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated for test purpose
</commit_message>
<xml_diff>
--- a/resources/testdata/TestSuite.xlsx
+++ b/resources/testdata/TestSuite.xlsx
@@ -392,7 +392,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +421,7 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -432,7 +432,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added xml for signup
</commit_message>
<xml_diff>
--- a/resources/testdata/TestSuite.xlsx
+++ b/resources/testdata/TestSuite.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>TSID</t>
   </si>
@@ -25,13 +25,19 @@
     <t>Runmode</t>
   </si>
   <si>
-    <t>Suite A for Regration</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
     <t>LoginTestCases</t>
+  </si>
+  <si>
+    <t>SignUpTestCases</t>
+  </si>
+  <si>
+    <t>Login Related Test cases</t>
+  </si>
+  <si>
+    <t>Self Registration Related Test Cases</t>
   </si>
 </sst>
 </file>
@@ -380,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,13 +412,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated for agent class
</commit_message>
<xml_diff>
--- a/resources/testdata/TestSuite.xlsx
+++ b/resources/testdata/TestSuite.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>TSID</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t>Self Registration Related Test Cases</t>
+  </si>
+  <si>
+    <t>AgentTestCases</t>
+  </si>
+  <si>
+    <t>Agent Related Test Cases</t>
   </si>
 </sst>
 </file>
@@ -386,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -432,6 +438,17 @@
         <v>3</v>
       </c>
     </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added test data for search and status test cases..
</commit_message>
<xml_diff>
--- a/resources/testdata/TestSuite.xlsx
+++ b/resources/testdata/TestSuite.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>TSID</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t>ResellerTests</t>
+  </si>
+  <si>
+    <t>UserSearchTestCase</t>
+  </si>
+  <si>
+    <t>UserStatusTestCase</t>
   </si>
 </sst>
 </file>
@@ -404,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,6 +486,22 @@
         <v>3</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixing failures. Refactoring Browser class and property reader in Config level context.
</commit_message>
<xml_diff>
--- a/resources/testdata/TestSuite.xlsx
+++ b/resources/testdata/TestSuite.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>TSID</t>
   </si>
@@ -62,21 +62,6 @@
   </si>
   <si>
     <t>UserStatusTestCase</t>
-  </si>
-  <si>
-    <t>SkippingTestCases</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Sample Skipping suit</t>
-  </si>
-  <si>
-    <t>SkippingSingleCase</t>
-  </si>
-  <si>
-    <t>Sample skipping test</t>
   </si>
 </sst>
 </file>
@@ -425,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,28 +502,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added for item bct
</commit_message>
<xml_diff>
--- a/resources/testdata/TestSuite.xlsx
+++ b/resources/testdata/TestSuite.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>TSID</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>BCT Cases For Item Module</t>
+  </si>
+  <si>
+    <t>ItemModuleBCT</t>
   </si>
 </sst>
 </file>
@@ -401,7 +407,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
@@ -469,6 +475,17 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
order placing tc and libs
</commit_message>
<xml_diff>
--- a/resources/testdata/TestSuite.xlsx
+++ b/resources/testdata/TestSuite.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>TSID</t>
   </si>
@@ -65,6 +65,9 @@
   </si>
   <si>
     <t>ItemModuleBCT</t>
+  </si>
+  <si>
+    <t>OrderTestCases</t>
   </si>
 </sst>
 </file>
@@ -413,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,6 +516,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Test data for regression
</commit_message>
<xml_diff>
--- a/resources/testdata/TestSuite.xlsx
+++ b/resources/testdata/TestSuite.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
   <si>
     <t>TSID</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>OrderTestCases</t>
+  </si>
+  <si>
+    <t>LoginScreenBugVerification</t>
   </si>
 </sst>
 </file>
@@ -416,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,6 +527,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>